<commit_message>
change filtering for teachers without roles to include admins
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/english.xlsx
+++ b/src/spz/templates/export/english.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="1" r:id="rId1"/>
@@ -1060,7 +1060,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:prstGeom prst="rect">
@@ -1546,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1913,7 +1912,7 @@
   </sheetPr>
   <dimension ref="A1:WWL70"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -5644,8 +5643,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showZeros="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5810,12 +5809,30 @@
       <c r="A5" s="40">
         <v>2</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="B5" s="41">
+        <f>RAWDATA!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="41">
+        <f>RAWDATA!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="42">
+        <f>RAWDATA!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="42">
+        <f>RAWDATA!E3</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="41">
+        <f>RAWDATA!I3</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="41">
+        <f>RAWDATA!J3</f>
+        <v>0</v>
+      </c>
       <c r="H5" s="42" t="str">
         <f>RAWDATA!K3</f>
         <v>Arabisch 1</v>
@@ -5849,12 +5866,30 @@
       <c r="A6" s="40">
         <v>3</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="41">
+        <f>RAWDATA!B4</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="41">
+        <f>RAWDATA!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="42">
+        <f>RAWDATA!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="42">
+        <f>RAWDATA!E4</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="41">
+        <f>RAWDATA!I4</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="41">
+        <f>RAWDATA!J4</f>
+        <v>0</v>
+      </c>
       <c r="H6" s="42" t="str">
         <f>RAWDATA!K4</f>
         <v>Arabisch 1</v>
@@ -5888,12 +5923,30 @@
       <c r="A7" s="40">
         <v>4</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="B7" s="41">
+        <f>RAWDATA!B5</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="41">
+        <f>RAWDATA!C5</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="42">
+        <f>RAWDATA!D5</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="42">
+        <f>RAWDATA!E5</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="41">
+        <f>RAWDATA!I5</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="41">
+        <f>RAWDATA!J5</f>
+        <v>0</v>
+      </c>
       <c r="H7" s="42" t="str">
         <f>RAWDATA!K5</f>
         <v>Arabisch 1</v>
@@ -5927,12 +5980,30 @@
       <c r="A8" s="40">
         <v>5</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="41">
+        <f>RAWDATA!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="41">
+        <f>RAWDATA!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="42">
+        <f>RAWDATA!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="42">
+        <f>RAWDATA!E6</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="41">
+        <f>RAWDATA!I6</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="41">
+        <f>RAWDATA!J6</f>
+        <v>0</v>
+      </c>
       <c r="H8" s="42" t="str">
         <f>RAWDATA!K6</f>
         <v>Arabisch 1</v>
@@ -5966,12 +6037,30 @@
       <c r="A9" s="40">
         <v>6</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="41">
+        <f>RAWDATA!B7</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="41">
+        <f>RAWDATA!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="42">
+        <f>RAWDATA!D7</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <f>RAWDATA!E7</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="41">
+        <f>RAWDATA!I7</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="41">
+        <f>RAWDATA!J7</f>
+        <v>0</v>
+      </c>
       <c r="H9" s="42" t="str">
         <f>RAWDATA!K7</f>
         <v>Arabisch 1</v>
@@ -6005,12 +6094,30 @@
       <c r="A10" s="40">
         <v>7</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="B10" s="41">
+        <f>RAWDATA!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="41">
+        <f>RAWDATA!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="42">
+        <f>RAWDATA!D8</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <f>RAWDATA!E8</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="41">
+        <f>RAWDATA!I8</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="41">
+        <f>RAWDATA!J8</f>
+        <v>0</v>
+      </c>
       <c r="H10" s="42" t="str">
         <f>RAWDATA!K8</f>
         <v>Arabisch 1</v>
@@ -6044,12 +6151,30 @@
       <c r="A11" s="40">
         <v>8</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="B11" s="41">
+        <f>RAWDATA!B9</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="41">
+        <f>RAWDATA!C9</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="42">
+        <f>RAWDATA!D9</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <f>RAWDATA!E9</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="41">
+        <f>RAWDATA!I9</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="41">
+        <f>RAWDATA!J9</f>
+        <v>0</v>
+      </c>
       <c r="H11" s="42" t="str">
         <f>RAWDATA!K9</f>
         <v>Arabisch 1</v>
@@ -6083,12 +6208,30 @@
       <c r="A12" s="40">
         <v>9</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="B12" s="41">
+        <f>RAWDATA!B10</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="41">
+        <f>RAWDATA!C10</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="42">
+        <f>RAWDATA!D10</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <f>RAWDATA!E10</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="41">
+        <f>RAWDATA!I10</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="41">
+        <f>RAWDATA!J10</f>
+        <v>0</v>
+      </c>
       <c r="H12" s="42" t="str">
         <f>RAWDATA!K10</f>
         <v>Arabisch 1</v>
@@ -6122,12 +6265,30 @@
       <c r="A13" s="40">
         <v>10</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="B13" s="41">
+        <f>RAWDATA!B11</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="41">
+        <f>RAWDATA!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="42">
+        <f>RAWDATA!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="42">
+        <f>RAWDATA!E11</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="41">
+        <f>RAWDATA!I11</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="41">
+        <f>RAWDATA!J11</f>
+        <v>0</v>
+      </c>
       <c r="H13" s="42" t="str">
         <f>RAWDATA!K11</f>
         <v>Arabisch 1</v>
@@ -6161,12 +6322,30 @@
       <c r="A14" s="40">
         <v>11</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="B14" s="41">
+        <f>RAWDATA!B12</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="41">
+        <f>RAWDATA!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="42">
+        <f>RAWDATA!D12</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="42">
+        <f>RAWDATA!E12</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="41">
+        <f>RAWDATA!I12</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="41">
+        <f>RAWDATA!J12</f>
+        <v>0</v>
+      </c>
       <c r="H14" s="42" t="str">
         <f>RAWDATA!K12</f>
         <v>Arabisch 1</v>
@@ -6200,12 +6379,30 @@
       <c r="A15" s="40">
         <v>12</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="B15" s="41">
+        <f>RAWDATA!B13</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="41">
+        <f>RAWDATA!C13</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="42">
+        <f>RAWDATA!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <f>RAWDATA!E13</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="41">
+        <f>RAWDATA!I13</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="41">
+        <f>RAWDATA!J13</f>
+        <v>0</v>
+      </c>
       <c r="H15" s="42" t="str">
         <f>RAWDATA!K13</f>
         <v>Arabisch 1</v>
@@ -6239,12 +6436,30 @@
       <c r="A16" s="40">
         <v>13</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="B16" s="41">
+        <f>RAWDATA!B14</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="41">
+        <f>RAWDATA!C14</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="42">
+        <f>RAWDATA!D14</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="42">
+        <f>RAWDATA!E14</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="41">
+        <f>RAWDATA!I14</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="41">
+        <f>RAWDATA!J14</f>
+        <v>0</v>
+      </c>
       <c r="H16" s="42" t="str">
         <f>RAWDATA!K14</f>
         <v>Arabisch 1</v>
@@ -6278,12 +6493,30 @@
       <c r="A17" s="40">
         <v>14</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
+      <c r="B17" s="41">
+        <f>RAWDATA!B15</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="41">
+        <f>RAWDATA!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="42">
+        <f>RAWDATA!D15</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="42">
+        <f>RAWDATA!E15</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="41">
+        <f>RAWDATA!I15</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="41">
+        <f>RAWDATA!J15</f>
+        <v>0</v>
+      </c>
       <c r="H17" s="42" t="str">
         <f>RAWDATA!K15</f>
         <v>Arabisch 1</v>
@@ -6317,12 +6550,30 @@
       <c r="A18" s="40">
         <v>15</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="B18" s="41">
+        <f>RAWDATA!B16</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="41">
+        <f>RAWDATA!C16</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="42">
+        <f>RAWDATA!D16</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="42">
+        <f>RAWDATA!E16</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="41">
+        <f>RAWDATA!I16</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="41">
+        <f>RAWDATA!J16</f>
+        <v>0</v>
+      </c>
       <c r="H18" s="42" t="str">
         <f>RAWDATA!K16</f>
         <v>Arabisch 1</v>
@@ -6356,12 +6607,30 @@
       <c r="A19" s="40">
         <v>16</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
+      <c r="B19" s="41">
+        <f>RAWDATA!B17</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="41">
+        <f>RAWDATA!C17</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="42">
+        <f>RAWDATA!D17</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="42">
+        <f>RAWDATA!E17</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="41">
+        <f>RAWDATA!I17</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="41">
+        <f>RAWDATA!J17</f>
+        <v>0</v>
+      </c>
       <c r="H19" s="42" t="str">
         <f>RAWDATA!K17</f>
         <v>Arabisch 1</v>
@@ -6395,12 +6664,30 @@
       <c r="A20" s="40">
         <v>17</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="B20" s="41">
+        <f>RAWDATA!B18</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="41">
+        <f>RAWDATA!C18</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="42">
+        <f>RAWDATA!D18</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="42">
+        <f>RAWDATA!E18</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="41">
+        <f>RAWDATA!I18</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="41">
+        <f>RAWDATA!J18</f>
+        <v>0</v>
+      </c>
       <c r="H20" s="42" t="str">
         <f>RAWDATA!K18</f>
         <v>Arabisch 1</v>
@@ -6434,12 +6721,30 @@
       <c r="A21" s="40">
         <v>18</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+      <c r="B21" s="41">
+        <f>RAWDATA!B19</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="41">
+        <f>RAWDATA!C19</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="42">
+        <f>RAWDATA!D19</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="42">
+        <f>RAWDATA!E19</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="41">
+        <f>RAWDATA!I19</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="41">
+        <f>RAWDATA!J19</f>
+        <v>0</v>
+      </c>
       <c r="H21" s="42" t="str">
         <f>RAWDATA!K19</f>
         <v>Arabisch 1</v>
@@ -6474,27 +6779,27 @@
         <v>19</v>
       </c>
       <c r="B22" s="41">
-        <f>RAWDATA!B3</f>
+        <f>RAWDATA!B20</f>
         <v>0</v>
       </c>
       <c r="C22" s="41">
-        <f>RAWDATA!C3</f>
+        <f>RAWDATA!C20</f>
         <v>0</v>
       </c>
       <c r="D22" s="42">
-        <f>RAWDATA!D3</f>
+        <f>RAWDATA!D20</f>
         <v>0</v>
       </c>
       <c r="E22" s="42">
-        <f>RAWDATA!E3</f>
+        <f>RAWDATA!E20</f>
         <v>0</v>
       </c>
       <c r="F22" s="41">
-        <f>RAWDATA!I3</f>
+        <f>RAWDATA!I20</f>
         <v>0</v>
       </c>
       <c r="G22" s="41">
-        <f>RAWDATA!J3</f>
+        <f>RAWDATA!J20</f>
         <v>0</v>
       </c>
       <c r="H22" s="42" t="str">
@@ -6531,27 +6836,27 @@
         <v>20</v>
       </c>
       <c r="B23" s="41">
-        <f>RAWDATA!B4</f>
+        <f>RAWDATA!B21</f>
         <v>0</v>
       </c>
       <c r="C23" s="41">
-        <f>RAWDATA!C4</f>
+        <f>RAWDATA!C21</f>
         <v>0</v>
       </c>
       <c r="D23" s="42">
-        <f>RAWDATA!D4</f>
+        <f>RAWDATA!D21</f>
         <v>0</v>
       </c>
       <c r="E23" s="42">
-        <f>RAWDATA!E4</f>
+        <f>RAWDATA!E21</f>
         <v>0</v>
       </c>
       <c r="F23" s="41">
-        <f>RAWDATA!I4</f>
+        <f>RAWDATA!I21</f>
         <v>0</v>
       </c>
       <c r="G23" s="41">
-        <f>RAWDATA!J4</f>
+        <f>RAWDATA!J21</f>
         <v>0</v>
       </c>
       <c r="H23" s="42" t="str">
@@ -6588,27 +6893,27 @@
         <v>21</v>
       </c>
       <c r="B24" s="41">
-        <f>RAWDATA!B5</f>
+        <f>RAWDATA!B22</f>
         <v>0</v>
       </c>
       <c r="C24" s="41">
-        <f>RAWDATA!C5</f>
+        <f>RAWDATA!C22</f>
         <v>0</v>
       </c>
       <c r="D24" s="42">
-        <f>RAWDATA!D5</f>
+        <f>RAWDATA!D22</f>
         <v>0</v>
       </c>
       <c r="E24" s="42">
-        <f>RAWDATA!E5</f>
+        <f>RAWDATA!E22</f>
         <v>0</v>
       </c>
       <c r="F24" s="41">
-        <f>RAWDATA!I5</f>
+        <f>RAWDATA!I22</f>
         <v>0</v>
       </c>
       <c r="G24" s="41">
-        <f>RAWDATA!J5</f>
+        <f>RAWDATA!J22</f>
         <v>0</v>
       </c>
       <c r="H24" s="42" t="str">
@@ -6645,27 +6950,27 @@
         <v>22</v>
       </c>
       <c r="B25" s="41">
-        <f>RAWDATA!B6</f>
+        <f>RAWDATA!B23</f>
         <v>0</v>
       </c>
       <c r="C25" s="41">
-        <f>RAWDATA!C6</f>
+        <f>RAWDATA!C23</f>
         <v>0</v>
       </c>
       <c r="D25" s="42">
-        <f>RAWDATA!D6</f>
+        <f>RAWDATA!D23</f>
         <v>0</v>
       </c>
       <c r="E25" s="42">
-        <f>RAWDATA!E6</f>
+        <f>RAWDATA!E23</f>
         <v>0</v>
       </c>
       <c r="F25" s="41">
-        <f>RAWDATA!I6</f>
+        <f>RAWDATA!I23</f>
         <v>0</v>
       </c>
       <c r="G25" s="41">
-        <f>RAWDATA!J6</f>
+        <f>RAWDATA!J23</f>
         <v>0</v>
       </c>
       <c r="H25" s="42" t="str">
@@ -6702,27 +7007,27 @@
         <v>23</v>
       </c>
       <c r="B26" s="41">
-        <f>RAWDATA!B7</f>
+        <f>RAWDATA!B24</f>
         <v>0</v>
       </c>
       <c r="C26" s="41">
-        <f>RAWDATA!C7</f>
+        <f>RAWDATA!C24</f>
         <v>0</v>
       </c>
       <c r="D26" s="42">
-        <f>RAWDATA!D7</f>
+        <f>RAWDATA!D24</f>
         <v>0</v>
       </c>
       <c r="E26" s="42">
-        <f>RAWDATA!E7</f>
+        <f>RAWDATA!E24</f>
         <v>0</v>
       </c>
       <c r="F26" s="41">
-        <f>RAWDATA!I7</f>
+        <f>RAWDATA!I24</f>
         <v>0</v>
       </c>
       <c r="G26" s="41">
-        <f>RAWDATA!J7</f>
+        <f>RAWDATA!J24</f>
         <v>0</v>
       </c>
       <c r="H26" s="42" t="str">
@@ -6759,27 +7064,27 @@
         <v>24</v>
       </c>
       <c r="B27" s="41">
-        <f>RAWDATA!B8</f>
+        <f>RAWDATA!B25</f>
         <v>0</v>
       </c>
       <c r="C27" s="41">
-        <f>RAWDATA!C8</f>
+        <f>RAWDATA!C25</f>
         <v>0</v>
       </c>
       <c r="D27" s="42">
-        <f>RAWDATA!D8</f>
+        <f>RAWDATA!D25</f>
         <v>0</v>
       </c>
       <c r="E27" s="42">
-        <f>RAWDATA!E8</f>
+        <f>RAWDATA!E25</f>
         <v>0</v>
       </c>
       <c r="F27" s="41">
-        <f>RAWDATA!I8</f>
+        <f>RAWDATA!I25</f>
         <v>0</v>
       </c>
       <c r="G27" s="41">
-        <f>RAWDATA!J8</f>
+        <f>RAWDATA!J25</f>
         <v>0</v>
       </c>
       <c r="H27" s="42">
@@ -6816,27 +7121,27 @@
         <v>25</v>
       </c>
       <c r="B28" s="41">
-        <f>RAWDATA!B9</f>
+        <f>RAWDATA!B26</f>
         <v>0</v>
       </c>
       <c r="C28" s="41">
-        <f>RAWDATA!C9</f>
+        <f>RAWDATA!C26</f>
         <v>0</v>
       </c>
       <c r="D28" s="42">
-        <f>RAWDATA!D9</f>
+        <f>RAWDATA!D26</f>
         <v>0</v>
       </c>
       <c r="E28" s="42">
-        <f>RAWDATA!E9</f>
+        <f>RAWDATA!E26</f>
         <v>0</v>
       </c>
       <c r="F28" s="41">
-        <f>RAWDATA!I9</f>
+        <f>RAWDATA!I26</f>
         <v>0</v>
       </c>
       <c r="G28" s="41">
-        <f>RAWDATA!J9</f>
+        <f>RAWDATA!J26</f>
         <v>0</v>
       </c>
       <c r="H28" s="42">
@@ -6873,27 +7178,27 @@
         <v>26</v>
       </c>
       <c r="B29" s="41">
-        <f>RAWDATA!B10</f>
+        <f>RAWDATA!B27</f>
         <v>0</v>
       </c>
       <c r="C29" s="41">
-        <f>RAWDATA!C10</f>
+        <f>RAWDATA!C27</f>
         <v>0</v>
       </c>
       <c r="D29" s="42">
-        <f>RAWDATA!D10</f>
+        <f>RAWDATA!D27</f>
         <v>0</v>
       </c>
       <c r="E29" s="42">
-        <f>RAWDATA!E10</f>
+        <f>RAWDATA!E27</f>
         <v>0</v>
       </c>
       <c r="F29" s="41">
-        <f>RAWDATA!I10</f>
+        <f>RAWDATA!I27</f>
         <v>0</v>
       </c>
       <c r="G29" s="41">
-        <f>RAWDATA!J10</f>
+        <f>RAWDATA!J27</f>
         <v>0</v>
       </c>
       <c r="H29" s="42">
@@ -6930,27 +7235,27 @@
         <v>27</v>
       </c>
       <c r="B30" s="41">
-        <f>RAWDATA!B11</f>
+        <f>RAWDATA!B28</f>
         <v>0</v>
       </c>
       <c r="C30" s="41">
-        <f>RAWDATA!C11</f>
+        <f>RAWDATA!C28</f>
         <v>0</v>
       </c>
       <c r="D30" s="42">
-        <f>RAWDATA!D11</f>
+        <f>RAWDATA!D28</f>
         <v>0</v>
       </c>
       <c r="E30" s="42">
-        <f>RAWDATA!E11</f>
+        <f>RAWDATA!E28</f>
         <v>0</v>
       </c>
       <c r="F30" s="41">
-        <f>RAWDATA!I11</f>
+        <f>RAWDATA!I28</f>
         <v>0</v>
       </c>
       <c r="G30" s="41">
-        <f>RAWDATA!J11</f>
+        <f>RAWDATA!J28</f>
         <v>0</v>
       </c>
       <c r="H30" s="42">
@@ -6987,27 +7292,27 @@
         <v>28</v>
       </c>
       <c r="B31" s="41">
-        <f>RAWDATA!B12</f>
+        <f>RAWDATA!B29</f>
         <v>0</v>
       </c>
       <c r="C31" s="41">
-        <f>RAWDATA!C12</f>
+        <f>RAWDATA!C29</f>
         <v>0</v>
       </c>
       <c r="D31" s="42">
-        <f>RAWDATA!D12</f>
+        <f>RAWDATA!D29</f>
         <v>0</v>
       </c>
       <c r="E31" s="42">
-        <f>RAWDATA!E12</f>
+        <f>RAWDATA!E29</f>
         <v>0</v>
       </c>
       <c r="F31" s="41">
-        <f>RAWDATA!I12</f>
+        <f>RAWDATA!I29</f>
         <v>0</v>
       </c>
       <c r="G31" s="41">
-        <f>RAWDATA!J12</f>
+        <f>RAWDATA!J29</f>
         <v>0</v>
       </c>
       <c r="H31" s="42">
@@ -7044,27 +7349,27 @@
         <v>29</v>
       </c>
       <c r="B32" s="41">
-        <f>RAWDATA!B13</f>
+        <f>RAWDATA!B30</f>
         <v>0</v>
       </c>
       <c r="C32" s="41">
-        <f>RAWDATA!C13</f>
+        <f>RAWDATA!C30</f>
         <v>0</v>
       </c>
       <c r="D32" s="42">
-        <f>RAWDATA!D13</f>
+        <f>RAWDATA!D30</f>
         <v>0</v>
       </c>
       <c r="E32" s="42">
-        <f>RAWDATA!E13</f>
+        <f>RAWDATA!E30</f>
         <v>0</v>
       </c>
       <c r="F32" s="41">
-        <f>RAWDATA!I13</f>
+        <f>RAWDATA!I30</f>
         <v>0</v>
       </c>
       <c r="G32" s="41">
-        <f>RAWDATA!J13</f>
+        <f>RAWDATA!J30</f>
         <v>0</v>
       </c>
       <c r="H32" s="42">
@@ -7101,27 +7406,27 @@
         <v>30</v>
       </c>
       <c r="B33" s="41">
-        <f>RAWDATA!B14</f>
+        <f>RAWDATA!B31</f>
         <v>0</v>
       </c>
       <c r="C33" s="41">
-        <f>RAWDATA!C14</f>
+        <f>RAWDATA!C31</f>
         <v>0</v>
       </c>
       <c r="D33" s="42">
-        <f>RAWDATA!D14</f>
+        <f>RAWDATA!D31</f>
         <v>0</v>
       </c>
       <c r="E33" s="42">
-        <f>RAWDATA!E14</f>
+        <f>RAWDATA!E31</f>
         <v>0</v>
       </c>
       <c r="F33" s="41">
-        <f>RAWDATA!I14</f>
+        <f>RAWDATA!I31</f>
         <v>0</v>
       </c>
       <c r="G33" s="41">
-        <f>RAWDATA!J14</f>
+        <f>RAWDATA!J31</f>
         <v>0</v>
       </c>
       <c r="H33" s="42">
@@ -7158,27 +7463,27 @@
         <v>31</v>
       </c>
       <c r="B34" s="41">
-        <f>RAWDATA!B15</f>
+        <f>RAWDATA!B32</f>
         <v>0</v>
       </c>
       <c r="C34" s="41">
-        <f>RAWDATA!C15</f>
+        <f>RAWDATA!C32</f>
         <v>0</v>
       </c>
       <c r="D34" s="42">
-        <f>RAWDATA!D15</f>
+        <f>RAWDATA!D32</f>
         <v>0</v>
       </c>
       <c r="E34" s="42">
-        <f>RAWDATA!E15</f>
+        <f>RAWDATA!E32</f>
         <v>0</v>
       </c>
       <c r="F34" s="41">
-        <f>RAWDATA!I15</f>
+        <f>RAWDATA!I32</f>
         <v>0</v>
       </c>
       <c r="G34" s="41">
-        <f>RAWDATA!J15</f>
+        <f>RAWDATA!J32</f>
         <v>0</v>
       </c>
       <c r="H34" s="42">
@@ -7215,27 +7520,27 @@
         <v>32</v>
       </c>
       <c r="B35" s="41">
-        <f>RAWDATA!B16</f>
+        <f>RAWDATA!B33</f>
         <v>0</v>
       </c>
       <c r="C35" s="41">
-        <f>RAWDATA!C16</f>
+        <f>RAWDATA!C33</f>
         <v>0</v>
       </c>
       <c r="D35" s="42">
-        <f>RAWDATA!D16</f>
+        <f>RAWDATA!D33</f>
         <v>0</v>
       </c>
       <c r="E35" s="42">
-        <f>RAWDATA!E16</f>
+        <f>RAWDATA!E33</f>
         <v>0</v>
       </c>
       <c r="F35" s="41">
-        <f>RAWDATA!I16</f>
+        <f>RAWDATA!I33</f>
         <v>0</v>
       </c>
       <c r="G35" s="41">
-        <f>RAWDATA!J16</f>
+        <f>RAWDATA!J33</f>
         <v>0</v>
       </c>
       <c r="H35" s="42">
@@ -7272,27 +7577,27 @@
         <v>33</v>
       </c>
       <c r="B36" s="41">
-        <f>RAWDATA!B17</f>
+        <f>RAWDATA!B34</f>
         <v>0</v>
       </c>
       <c r="C36" s="41">
-        <f>RAWDATA!C17</f>
+        <f>RAWDATA!C34</f>
         <v>0</v>
       </c>
       <c r="D36" s="42">
-        <f>RAWDATA!D17</f>
+        <f>RAWDATA!D34</f>
         <v>0</v>
       </c>
       <c r="E36" s="42">
-        <f>RAWDATA!E17</f>
+        <f>RAWDATA!E34</f>
         <v>0</v>
       </c>
       <c r="F36" s="41">
-        <f>RAWDATA!I17</f>
+        <f>RAWDATA!I34</f>
         <v>0</v>
       </c>
       <c r="G36" s="41">
-        <f>RAWDATA!J17</f>
+        <f>RAWDATA!J34</f>
         <v>0</v>
       </c>
       <c r="H36" s="42">
@@ -7329,27 +7634,27 @@
         <v>34</v>
       </c>
       <c r="B37" s="41">
-        <f>RAWDATA!B18</f>
+        <f>RAWDATA!B35</f>
         <v>0</v>
       </c>
       <c r="C37" s="41">
-        <f>RAWDATA!C18</f>
+        <f>RAWDATA!C35</f>
         <v>0</v>
       </c>
       <c r="D37" s="42">
-        <f>RAWDATA!D18</f>
+        <f>RAWDATA!D35</f>
         <v>0</v>
       </c>
       <c r="E37" s="42">
-        <f>RAWDATA!E18</f>
+        <f>RAWDATA!E35</f>
         <v>0</v>
       </c>
       <c r="F37" s="41">
-        <f>RAWDATA!I18</f>
+        <f>RAWDATA!I35</f>
         <v>0</v>
       </c>
       <c r="G37" s="41">
-        <f>RAWDATA!J18</f>
+        <f>RAWDATA!J35</f>
         <v>0</v>
       </c>
       <c r="H37" s="42">
@@ -7386,27 +7691,27 @@
         <v>35</v>
       </c>
       <c r="B38" s="41">
-        <f>RAWDATA!B19</f>
+        <f>RAWDATA!B36</f>
         <v>0</v>
       </c>
       <c r="C38" s="41">
-        <f>RAWDATA!C19</f>
+        <f>RAWDATA!C36</f>
         <v>0</v>
       </c>
       <c r="D38" s="42">
-        <f>RAWDATA!D19</f>
+        <f>RAWDATA!D36</f>
         <v>0</v>
       </c>
       <c r="E38" s="42">
-        <f>RAWDATA!E19</f>
+        <f>RAWDATA!E36</f>
         <v>0</v>
       </c>
       <c r="F38" s="41">
-        <f>RAWDATA!I19</f>
+        <f>RAWDATA!I36</f>
         <v>0</v>
       </c>
       <c r="G38" s="41">
-        <f>RAWDATA!J19</f>
+        <f>RAWDATA!J36</f>
         <v>0</v>
       </c>
       <c r="H38" s="42">
@@ -7566,8 +7871,8 @@
   </sheetPr>
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E23"/>
+    <sheetView showZeros="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -7814,10 +8119,22 @@
       <c r="A7" s="40">
         <v>2</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="41">
+        <f>RAWDATA!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="41">
+        <f>RAWDATA!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="41">
+        <f>RAWDATA!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="41">
+        <f>RAWDATA!E3</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="56"/>
       <c r="G7" s="57"/>
       <c r="H7" s="57"/>
@@ -7842,10 +8159,22 @@
       <c r="A8" s="40">
         <v>3</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="B8" s="41">
+        <f>RAWDATA!B4</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="41">
+        <f>RAWDATA!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="41">
+        <f>RAWDATA!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="41">
+        <f>RAWDATA!E4</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="56"/>
       <c r="G8" s="57"/>
       <c r="H8" s="57"/>
@@ -7870,10 +8199,22 @@
       <c r="A9" s="40">
         <v>4</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="B9" s="41">
+        <f>RAWDATA!B5</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="41">
+        <f>RAWDATA!C5</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="41">
+        <f>RAWDATA!D5</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="41">
+        <f>RAWDATA!E5</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="56"/>
       <c r="G9" s="57"/>
       <c r="H9" s="57"/>
@@ -7898,10 +8239,22 @@
       <c r="A10" s="40">
         <v>5</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="B10" s="41">
+        <f>RAWDATA!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="41">
+        <f>RAWDATA!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="41">
+        <f>RAWDATA!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="41">
+        <f>RAWDATA!E6</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="56"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
@@ -7926,10 +8279,22 @@
       <c r="A11" s="40">
         <v>6</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="41">
+        <f>RAWDATA!B7</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="41">
+        <f>RAWDATA!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="41">
+        <f>RAWDATA!D7</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="41">
+        <f>RAWDATA!E7</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
       <c r="H11" s="57"/>
@@ -7954,10 +8319,22 @@
       <c r="A12" s="40">
         <v>7</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="41">
+        <f>RAWDATA!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="41">
+        <f>RAWDATA!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="41">
+        <f>RAWDATA!D8</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="41">
+        <f>RAWDATA!E8</f>
+        <v>0</v>
+      </c>
       <c r="F12" s="56"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
@@ -7982,10 +8359,22 @@
       <c r="A13" s="40">
         <v>8</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="B13" s="41">
+        <f>RAWDATA!B9</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="41">
+        <f>RAWDATA!C9</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <f>RAWDATA!D9</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="41">
+        <f>RAWDATA!E9</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="56"/>
       <c r="G13" s="57"/>
       <c r="H13" s="57"/>
@@ -8010,10 +8399,22 @@
       <c r="A14" s="40">
         <v>9</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="B14" s="41">
+        <f>RAWDATA!B10</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="41">
+        <f>RAWDATA!C10</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="41">
+        <f>RAWDATA!D10</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="41">
+        <f>RAWDATA!E10</f>
+        <v>0</v>
+      </c>
       <c r="F14" s="56"/>
       <c r="G14" s="57"/>
       <c r="H14" s="57"/>
@@ -8038,10 +8439,22 @@
       <c r="A15" s="40">
         <v>10</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="41">
+        <f>RAWDATA!B11</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="41">
+        <f>RAWDATA!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="41">
+        <f>RAWDATA!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="41">
+        <f>RAWDATA!E11</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="56"/>
       <c r="G15" s="57"/>
       <c r="H15" s="57"/>
@@ -8066,10 +8479,22 @@
       <c r="A16" s="40">
         <v>11</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="41">
+        <f>RAWDATA!B12</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="41">
+        <f>RAWDATA!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="41">
+        <f>RAWDATA!D12</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="41">
+        <f>RAWDATA!E12</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="56"/>
       <c r="G16" s="57"/>
       <c r="H16" s="57"/>
@@ -8094,10 +8519,22 @@
       <c r="A17" s="40">
         <v>12</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="41">
+        <f>RAWDATA!B13</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="41">
+        <f>RAWDATA!C13</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="41">
+        <f>RAWDATA!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="41">
+        <f>RAWDATA!E13</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="56"/>
       <c r="G17" s="57"/>
       <c r="H17" s="57"/>
@@ -8122,10 +8559,22 @@
       <c r="A18" s="40">
         <v>13</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="B18" s="41">
+        <f>RAWDATA!B14</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="41">
+        <f>RAWDATA!C14</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="41">
+        <f>RAWDATA!D14</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="41">
+        <f>RAWDATA!E14</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="56"/>
       <c r="G18" s="57"/>
       <c r="H18" s="57"/>
@@ -8150,10 +8599,22 @@
       <c r="A19" s="40">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="41">
+        <f>RAWDATA!B15</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="41">
+        <f>RAWDATA!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="41">
+        <f>RAWDATA!D15</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="41">
+        <f>RAWDATA!E15</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="56"/>
       <c r="G19" s="57"/>
       <c r="H19" s="57"/>
@@ -8178,10 +8639,22 @@
       <c r="A20" s="40">
         <v>15</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="B20" s="41">
+        <f>RAWDATA!B16</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="41">
+        <f>RAWDATA!C16</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="41">
+        <f>RAWDATA!D16</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="41">
+        <f>RAWDATA!E16</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="56"/>
       <c r="G20" s="57"/>
       <c r="H20" s="57"/>
@@ -8206,10 +8679,22 @@
       <c r="A21" s="40">
         <v>16</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="B21" s="41">
+        <f>RAWDATA!B17</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="41">
+        <f>RAWDATA!C17</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="41">
+        <f>RAWDATA!D17</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="41">
+        <f>RAWDATA!E17</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="56"/>
       <c r="G21" s="57"/>
       <c r="H21" s="57"/>
@@ -8234,10 +8719,22 @@
       <c r="A22" s="40">
         <v>17</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="41">
+        <f>RAWDATA!B18</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="41">
+        <f>RAWDATA!C18</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="41">
+        <f>RAWDATA!D18</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="41">
+        <f>RAWDATA!E18</f>
+        <v>0</v>
+      </c>
       <c r="F22" s="56"/>
       <c r="G22" s="57"/>
       <c r="H22" s="57"/>
@@ -8262,10 +8759,22 @@
       <c r="A23" s="40">
         <v>18</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="B23" s="41">
+        <f>RAWDATA!B19</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="41">
+        <f>RAWDATA!C19</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="41">
+        <f>RAWDATA!D19</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="41">
+        <f>RAWDATA!E19</f>
+        <v>0</v>
+      </c>
       <c r="F23" s="56"/>
       <c r="G23" s="57"/>
       <c r="H23" s="57"/>
@@ -8291,19 +8800,19 @@
         <v>19</v>
       </c>
       <c r="B24" s="41">
-        <f>RAWDATA!B3</f>
+        <f>RAWDATA!B20</f>
         <v>0</v>
       </c>
       <c r="C24" s="41">
-        <f>RAWDATA!C3</f>
+        <f>RAWDATA!C20</f>
         <v>0</v>
       </c>
       <c r="D24" s="41">
-        <f>RAWDATA!D3</f>
+        <f>RAWDATA!D20</f>
         <v>0</v>
       </c>
       <c r="E24" s="41">
-        <f>RAWDATA!E3</f>
+        <f>RAWDATA!E20</f>
         <v>0</v>
       </c>
       <c r="F24" s="56"/>
@@ -8331,19 +8840,19 @@
         <v>20</v>
       </c>
       <c r="B25" s="41">
-        <f>RAWDATA!B4</f>
+        <f>RAWDATA!B21</f>
         <v>0</v>
       </c>
       <c r="C25" s="41">
-        <f>RAWDATA!C4</f>
+        <f>RAWDATA!C21</f>
         <v>0</v>
       </c>
       <c r="D25" s="41">
-        <f>RAWDATA!D4</f>
+        <f>RAWDATA!D21</f>
         <v>0</v>
       </c>
       <c r="E25" s="41">
-        <f>RAWDATA!E4</f>
+        <f>RAWDATA!E21</f>
         <v>0</v>
       </c>
       <c r="F25" s="56"/>
@@ -8371,19 +8880,19 @@
         <v>21</v>
       </c>
       <c r="B26" s="41">
-        <f>RAWDATA!B5</f>
+        <f>RAWDATA!B22</f>
         <v>0</v>
       </c>
       <c r="C26" s="41">
-        <f>RAWDATA!C5</f>
+        <f>RAWDATA!C22</f>
         <v>0</v>
       </c>
       <c r="D26" s="41">
-        <f>RAWDATA!D5</f>
+        <f>RAWDATA!D22</f>
         <v>0</v>
       </c>
       <c r="E26" s="41">
-        <f>RAWDATA!E5</f>
+        <f>RAWDATA!E22</f>
         <v>0</v>
       </c>
       <c r="F26" s="56"/>
@@ -8411,19 +8920,19 @@
         <v>22</v>
       </c>
       <c r="B27" s="41">
-        <f>RAWDATA!B6</f>
+        <f>RAWDATA!B23</f>
         <v>0</v>
       </c>
       <c r="C27" s="41">
-        <f>RAWDATA!C6</f>
+        <f>RAWDATA!C23</f>
         <v>0</v>
       </c>
       <c r="D27" s="41">
-        <f>RAWDATA!D6</f>
+        <f>RAWDATA!D23</f>
         <v>0</v>
       </c>
       <c r="E27" s="41">
-        <f>RAWDATA!E6</f>
+        <f>RAWDATA!E23</f>
         <v>0</v>
       </c>
       <c r="F27" s="56"/>
@@ -8451,19 +8960,19 @@
         <v>23</v>
       </c>
       <c r="B28" s="41">
-        <f>RAWDATA!B7</f>
+        <f>RAWDATA!B24</f>
         <v>0</v>
       </c>
       <c r="C28" s="41">
-        <f>RAWDATA!C7</f>
+        <f>RAWDATA!C24</f>
         <v>0</v>
       </c>
       <c r="D28" s="41">
-        <f>RAWDATA!D7</f>
+        <f>RAWDATA!D24</f>
         <v>0</v>
       </c>
       <c r="E28" s="41">
-        <f>RAWDATA!E7</f>
+        <f>RAWDATA!E24</f>
         <v>0</v>
       </c>
       <c r="F28" s="56"/>
@@ -8491,19 +9000,19 @@
         <v>24</v>
       </c>
       <c r="B29" s="41">
-        <f>RAWDATA!B8</f>
+        <f>RAWDATA!B25</f>
         <v>0</v>
       </c>
       <c r="C29" s="41">
-        <f>RAWDATA!C8</f>
+        <f>RAWDATA!C25</f>
         <v>0</v>
       </c>
       <c r="D29" s="41">
-        <f>RAWDATA!D8</f>
+        <f>RAWDATA!D25</f>
         <v>0</v>
       </c>
       <c r="E29" s="41">
-        <f>RAWDATA!E8</f>
+        <f>RAWDATA!E25</f>
         <v>0</v>
       </c>
       <c r="F29" s="56"/>
@@ -8531,19 +9040,19 @@
         <v>25</v>
       </c>
       <c r="B30" s="41">
-        <f>RAWDATA!B9</f>
+        <f>RAWDATA!B26</f>
         <v>0</v>
       </c>
       <c r="C30" s="41">
-        <f>RAWDATA!C9</f>
+        <f>RAWDATA!C26</f>
         <v>0</v>
       </c>
       <c r="D30" s="41">
-        <f>RAWDATA!D9</f>
+        <f>RAWDATA!D26</f>
         <v>0</v>
       </c>
       <c r="E30" s="41">
-        <f>RAWDATA!E9</f>
+        <f>RAWDATA!E26</f>
         <v>0</v>
       </c>
       <c r="F30" s="56"/>
@@ -8571,19 +9080,19 @@
         <v>26</v>
       </c>
       <c r="B31" s="41">
-        <f>RAWDATA!B10</f>
+        <f>RAWDATA!B27</f>
         <v>0</v>
       </c>
       <c r="C31" s="41">
-        <f>RAWDATA!C10</f>
+        <f>RAWDATA!C27</f>
         <v>0</v>
       </c>
       <c r="D31" s="41">
-        <f>RAWDATA!D10</f>
+        <f>RAWDATA!D27</f>
         <v>0</v>
       </c>
       <c r="E31" s="41">
-        <f>RAWDATA!E10</f>
+        <f>RAWDATA!E27</f>
         <v>0</v>
       </c>
       <c r="F31" s="56"/>
@@ -8611,19 +9120,19 @@
         <v>27</v>
       </c>
       <c r="B32" s="41">
-        <f>RAWDATA!B11</f>
+        <f>RAWDATA!B28</f>
         <v>0</v>
       </c>
       <c r="C32" s="41">
-        <f>RAWDATA!C11</f>
+        <f>RAWDATA!C28</f>
         <v>0</v>
       </c>
       <c r="D32" s="41">
-        <f>RAWDATA!D11</f>
+        <f>RAWDATA!D28</f>
         <v>0</v>
       </c>
       <c r="E32" s="41">
-        <f>RAWDATA!E11</f>
+        <f>RAWDATA!E28</f>
         <v>0</v>
       </c>
       <c r="F32" s="56"/>
@@ -8651,19 +9160,19 @@
         <v>28</v>
       </c>
       <c r="B33" s="41">
-        <f>RAWDATA!B12</f>
+        <f>RAWDATA!B29</f>
         <v>0</v>
       </c>
       <c r="C33" s="41">
-        <f>RAWDATA!C12</f>
+        <f>RAWDATA!C29</f>
         <v>0</v>
       </c>
       <c r="D33" s="41">
-        <f>RAWDATA!D12</f>
+        <f>RAWDATA!D29</f>
         <v>0</v>
       </c>
       <c r="E33" s="41">
-        <f>RAWDATA!E12</f>
+        <f>RAWDATA!E29</f>
         <v>0</v>
       </c>
       <c r="F33" s="56"/>
@@ -8691,19 +9200,19 @@
         <v>29</v>
       </c>
       <c r="B34" s="41">
-        <f>RAWDATA!B13</f>
+        <f>RAWDATA!B30</f>
         <v>0</v>
       </c>
       <c r="C34" s="41">
-        <f>RAWDATA!C13</f>
+        <f>RAWDATA!C30</f>
         <v>0</v>
       </c>
       <c r="D34" s="41">
-        <f>RAWDATA!D13</f>
+        <f>RAWDATA!D30</f>
         <v>0</v>
       </c>
       <c r="E34" s="41">
-        <f>RAWDATA!E13</f>
+        <f>RAWDATA!E30</f>
         <v>0</v>
       </c>
       <c r="F34" s="56"/>
@@ -8731,19 +9240,19 @@
         <v>30</v>
       </c>
       <c r="B35" s="41">
-        <f>RAWDATA!B14</f>
+        <f>RAWDATA!B31</f>
         <v>0</v>
       </c>
       <c r="C35" s="41">
-        <f>RAWDATA!C14</f>
+        <f>RAWDATA!C31</f>
         <v>0</v>
       </c>
       <c r="D35" s="41">
-        <f>RAWDATA!D14</f>
+        <f>RAWDATA!D31</f>
         <v>0</v>
       </c>
       <c r="E35" s="41">
-        <f>RAWDATA!E14</f>
+        <f>RAWDATA!E31</f>
         <v>0</v>
       </c>
       <c r="F35" s="56"/>
@@ -8771,19 +9280,19 @@
         <v>31</v>
       </c>
       <c r="B36" s="41">
-        <f>RAWDATA!B15</f>
+        <f>RAWDATA!B32</f>
         <v>0</v>
       </c>
       <c r="C36" s="41">
-        <f>RAWDATA!C15</f>
+        <f>RAWDATA!C32</f>
         <v>0</v>
       </c>
       <c r="D36" s="41">
-        <f>RAWDATA!D15</f>
+        <f>RAWDATA!D32</f>
         <v>0</v>
       </c>
       <c r="E36" s="41">
-        <f>RAWDATA!E15</f>
+        <f>RAWDATA!E32</f>
         <v>0</v>
       </c>
       <c r="F36" s="56"/>
@@ -8811,19 +9320,19 @@
         <v>32</v>
       </c>
       <c r="B37" s="41">
-        <f>RAWDATA!B16</f>
+        <f>RAWDATA!B33</f>
         <v>0</v>
       </c>
       <c r="C37" s="41">
-        <f>RAWDATA!C16</f>
+        <f>RAWDATA!C33</f>
         <v>0</v>
       </c>
       <c r="D37" s="41">
-        <f>RAWDATA!D16</f>
+        <f>RAWDATA!D33</f>
         <v>0</v>
       </c>
       <c r="E37" s="41">
-        <f>RAWDATA!E16</f>
+        <f>RAWDATA!E33</f>
         <v>0</v>
       </c>
       <c r="F37" s="56"/>
@@ -8851,19 +9360,19 @@
         <v>33</v>
       </c>
       <c r="B38" s="41">
-        <f>RAWDATA!B17</f>
+        <f>RAWDATA!B34</f>
         <v>0</v>
       </c>
       <c r="C38" s="41">
-        <f>RAWDATA!C17</f>
+        <f>RAWDATA!C34</f>
         <v>0</v>
       </c>
       <c r="D38" s="41">
-        <f>RAWDATA!D17</f>
+        <f>RAWDATA!D34</f>
         <v>0</v>
       </c>
       <c r="E38" s="41">
-        <f>RAWDATA!E17</f>
+        <f>RAWDATA!E34</f>
         <v>0</v>
       </c>
       <c r="F38" s="56"/>
@@ -8891,19 +9400,19 @@
         <v>34</v>
       </c>
       <c r="B39" s="41">
-        <f>RAWDATA!B18</f>
+        <f>RAWDATA!B35</f>
         <v>0</v>
       </c>
       <c r="C39" s="41">
-        <f>RAWDATA!C18</f>
+        <f>RAWDATA!C35</f>
         <v>0</v>
       </c>
       <c r="D39" s="41">
-        <f>RAWDATA!D18</f>
+        <f>RAWDATA!D35</f>
         <v>0</v>
       </c>
       <c r="E39" s="41">
-        <f>RAWDATA!E18</f>
+        <f>RAWDATA!E35</f>
         <v>0</v>
       </c>
       <c r="F39" s="56"/>
@@ -8931,19 +9440,19 @@
         <v>35</v>
       </c>
       <c r="B40" s="41">
-        <f>RAWDATA!B19</f>
+        <f>RAWDATA!B36</f>
         <v>0</v>
       </c>
       <c r="C40" s="41">
-        <f>RAWDATA!C19</f>
+        <f>RAWDATA!C36</f>
         <v>0</v>
       </c>
       <c r="D40" s="41">
-        <f>RAWDATA!D19</f>
+        <f>RAWDATA!D36</f>
         <v>0</v>
       </c>
       <c r="E40" s="41">
-        <f>RAWDATA!E19</f>
+        <f>RAWDATA!E36</f>
         <v>0</v>
       </c>
       <c r="F40" s="56"/>

</xml_diff>